<commit_message>
Fotos da festinha de ontem
</commit_message>
<xml_diff>
--- a/Dados Graficos.xlsx
+++ b/Dados Graficos.xlsx
@@ -157,11 +157,11 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,11 +565,11 @@
         </c:dLbls>
         <c:gapWidth val="164"/>
         <c:overlap val="-22"/>
-        <c:axId val="1437309744"/>
-        <c:axId val="1437311920"/>
+        <c:axId val="-802435440"/>
+        <c:axId val="-762778848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1437309744"/>
+        <c:axId val="-802435440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +612,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437311920"/>
+        <c:crossAx val="-762778848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1437311920"/>
+        <c:axId val="-762778848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437309744"/>
+        <c:crossAx val="-802435440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1118,11 +1118,11 @@
         </c:dLbls>
         <c:gapWidth val="164"/>
         <c:overlap val="-22"/>
-        <c:axId val="1437309200"/>
-        <c:axId val="1437310288"/>
+        <c:axId val="-762783744"/>
+        <c:axId val="-762785376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1437309200"/>
+        <c:axId val="-762783744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1165,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437310288"/>
+        <c:crossAx val="-762785376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1173,7 +1173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1437310288"/>
+        <c:axId val="-762785376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1210,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437309200"/>
+        <c:crossAx val="-762783744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1671,11 +1671,11 @@
         </c:dLbls>
         <c:gapWidth val="164"/>
         <c:overlap val="-22"/>
-        <c:axId val="1437301584"/>
-        <c:axId val="1437297776"/>
+        <c:axId val="-762774496"/>
+        <c:axId val="-762772320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1437301584"/>
+        <c:axId val="-762774496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1718,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437297776"/>
+        <c:crossAx val="-762772320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1726,7 +1726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1437297776"/>
+        <c:axId val="-762772320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1763,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437301584"/>
+        <c:crossAx val="-762774496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,11 +2224,11 @@
         </c:dLbls>
         <c:gapWidth val="164"/>
         <c:overlap val="-22"/>
-        <c:axId val="1437299952"/>
-        <c:axId val="1437305936"/>
+        <c:axId val="-762777216"/>
+        <c:axId val="-762773408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1437299952"/>
+        <c:axId val="-762777216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,7 +2271,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437305936"/>
+        <c:crossAx val="-762773408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2279,7 +2279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1437305936"/>
+        <c:axId val="-762773408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2316,7 +2316,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1437299952"/>
+        <c:crossAx val="-762777216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2558,11 +2558,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1530684176"/>
-        <c:axId val="1530685264"/>
+        <c:axId val="-762776128"/>
+        <c:axId val="-762771776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1530684176"/>
+        <c:axId val="-762776128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2605,7 +2605,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530685264"/>
+        <c:crossAx val="-762771776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2613,7 +2613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1530685264"/>
+        <c:axId val="-762771776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,7 +2664,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530684176"/>
+        <c:crossAx val="-762776128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2874,11 +2874,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1530687440"/>
-        <c:axId val="1530690160"/>
+        <c:axId val="-762779936"/>
+        <c:axId val="-762779392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1530687440"/>
+        <c:axId val="-762779936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,7 +2921,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530690160"/>
+        <c:crossAx val="-762779392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2929,7 +2929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1530690160"/>
+        <c:axId val="-762779392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +2980,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530687440"/>
+        <c:crossAx val="-762779936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3196,11 +3196,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1530684720"/>
-        <c:axId val="1530687984"/>
+        <c:axId val="-762781568"/>
+        <c:axId val="-762786464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1530684720"/>
+        <c:axId val="-762781568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3243,7 +3243,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530687984"/>
+        <c:crossAx val="-762786464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3251,7 +3251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1530687984"/>
+        <c:axId val="-762786464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3302,7 +3302,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1530684720"/>
+        <c:crossAx val="-762781568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3512,11 +3512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1277742144"/>
-        <c:axId val="1277746496"/>
+        <c:axId val="-762775584"/>
+        <c:axId val="-762785920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1277742144"/>
+        <c:axId val="-762775584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3559,7 +3559,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277746496"/>
+        <c:crossAx val="-762785920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3567,7 +3567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1277746496"/>
+        <c:axId val="-762785920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3618,7 +3618,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277742144"/>
+        <c:crossAx val="-762775584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3632,6 +3632,342 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Utilização - Link de Saída</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Plan1!$B$31:$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Observação 1 (80)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Observação 2 (0.8)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Observação 3 (5.5)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Observação 4 (800)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Observação 5 (22,23)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$38:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1176</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.58E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7100000000000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-638113360"/>
+        <c:axId val="-638101936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-638113360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-638101936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-638101936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-638113360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -3987,6 +4323,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
@@ -7612,6 +7988,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8375,6 +9267,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1860176</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>169209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1479176</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>54909</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8643,8 +9565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8690,7 +9612,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -8823,14 +9745,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -8966,14 +9888,14 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -9106,14 +10028,14 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -9244,12 +10166,12 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
@@ -9345,19 +10267,19 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <v>0.1176</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="10">
         <v>4.58E-2</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="10">
         <v>0.60899999999999999</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="10">
         <v>7.7100000000000002E-2</v>
       </c>
     </row>
@@ -9434,7 +10356,7 @@
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50"/>
       <c r="D50"/>
-      <c r="E50"/>
+      <c r="E50" s="8"/>
       <c r="F50"/>
       <c r="H50"/>
     </row>

</xml_diff>